<commit_message>
aspiration example set up
</commit_message>
<xml_diff>
--- a/examples/Aspiration/data/excel_source/GA_training_scenarios.xlsx
+++ b/examples/Aspiration/data/excel_source/GA_training_scenarios.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>training_generation</t>
   </si>
@@ -33,9 +34,6 @@
     <t>id_training_scenario</t>
   </si>
   <si>
-    <t>number_of_training_path</t>
-  </si>
-  <si>
     <t>strategy_param_code_length</t>
   </si>
   <si>
@@ -55,6 +53,30 @@
   </si>
   <si>
     <t>strategy_param_3_max</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>number_of_path</t>
+  </si>
+  <si>
+    <t>id_scenario</t>
+  </si>
+  <si>
+    <t>id_agent</t>
+  </si>
+  <si>
+    <t>strategy_param_1</t>
+  </si>
+  <si>
+    <t>strategy_param_2</t>
+  </si>
+  <si>
+    <t>strategy_param_3</t>
+  </si>
+  <si>
+    <t>id_path</t>
   </si>
 </sst>
 </file>
@@ -375,31 +397,31 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -411,28 +433,28 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -470,7 +492,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -506,6 +528,50 @@
       </c>
       <c r="L3">
         <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>